<commit_message>
With new test case
</commit_message>
<xml_diff>
--- a/testData/Opencart_LoginData.xlsx
+++ b/testData/Opencart_LoginData.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Automation\Myworkspace\OpenCart_Framework\testData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Automation\Myworkspace\opencart_v121\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B71A412-FD01-4366-8996-4F1DDC75DEE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{865642F1-365A-43C7-962F-1C1B8D0F4181}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{1F2D179E-37D2-4BC0-88A9-F5C135B87DA5}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="15">
   <si>
     <t>username</t>
   </si>
@@ -39,13 +39,7 @@
     <t>lakshmi@yahoo.com</t>
   </si>
   <si>
-    <t>Lakshmi</t>
-  </si>
-  <si>
     <t>Valid</t>
-  </si>
-  <si>
-    <t>laksh@yahoo.com</t>
   </si>
   <si>
     <t>Laxmi</t>
@@ -494,7 +488,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -517,13 +511,13 @@
     </row>
     <row r="2" spans="1:3" ht="21" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="21" x14ac:dyDescent="0.4">
@@ -531,88 +525,83 @@
         <v>3</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="21" x14ac:dyDescent="0.4">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="2"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3" t="s">
         <v>6</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="21" x14ac:dyDescent="0.4">
       <c r="A5" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="21" x14ac:dyDescent="0.4">
       <c r="A6" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="21" x14ac:dyDescent="0.4">
       <c r="A7" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="21" x14ac:dyDescent="0.4">
       <c r="A8" s="2"/>
       <c r="B8" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="21" x14ac:dyDescent="0.4">
       <c r="A9" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B9" s="4"/>
       <c r="C9" s="3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{D3BE7519-95C3-4ACD-9AB4-5385C9508082}"/>
-    <hyperlink ref="A4" r:id="rId2" xr:uid="{8456409A-CACC-4B7E-B78E-75E713148E0E}"/>
-    <hyperlink ref="A3" r:id="rId3" xr:uid="{5E52A498-5B14-4BDC-BBF1-05425B8AC197}"/>
-    <hyperlink ref="A5" r:id="rId4" xr:uid="{94E9D5A6-98A1-4A25-BDDE-C5B20EDA887E}"/>
-    <hyperlink ref="B2" r:id="rId5" xr:uid="{968262D0-AE14-41EF-AB8A-08B3F886E797}"/>
-    <hyperlink ref="A6" r:id="rId6" xr:uid="{75A4F8D6-7BF1-446B-9367-475FA4FB44C7}"/>
-    <hyperlink ref="B6" r:id="rId7" xr:uid="{01D5649A-5E55-45E1-9B81-1CE430C208A1}"/>
-    <hyperlink ref="A7" r:id="rId8" xr:uid="{51C37285-4E8C-489A-819E-D71A93634CC0}"/>
-    <hyperlink ref="B7" r:id="rId9" xr:uid="{B7516E5F-BE06-4C4C-843A-22073C8B9235}"/>
+    <hyperlink ref="A3" r:id="rId2" xr:uid="{5E52A498-5B14-4BDC-BBF1-05425B8AC197}"/>
+    <hyperlink ref="A5" r:id="rId3" xr:uid="{94E9D5A6-98A1-4A25-BDDE-C5B20EDA887E}"/>
+    <hyperlink ref="B2" r:id="rId4" xr:uid="{968262D0-AE14-41EF-AB8A-08B3F886E797}"/>
+    <hyperlink ref="A6" r:id="rId5" xr:uid="{75A4F8D6-7BF1-446B-9367-475FA4FB44C7}"/>
+    <hyperlink ref="B6" r:id="rId6" xr:uid="{01D5649A-5E55-45E1-9B81-1CE430C208A1}"/>
+    <hyperlink ref="A7" r:id="rId7" xr:uid="{51C37285-4E8C-489A-819E-D71A93634CC0}"/>
+    <hyperlink ref="B7" r:id="rId8" xr:uid="{B7516E5F-BE06-4C4C-843A-22073C8B9235}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId10"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId9"/>
 </worksheet>
 </file>
</xml_diff>